<commit_message>
adding two test datasets that we want to run triples on, also cleaned up ppo_config to accomodate slight changes in these files
</commit_message>
<xml_diff>
--- a/docs/fims/neon_example/single.xlsx
+++ b/docs/fims/neon_example/single.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdeck/tmp/PPO/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jdeck/IdeaProjects/PPO/docs/fims/neon_example/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -413,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD7"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -423,13 +423,14 @@
     <col min="2" max="2" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.83203125" customWidth="1"/>
+    <col min="7" max="10" width="0" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="20" customWidth="1"/>
     <col min="13" max="13" width="21.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.6640625" customWidth="1"/>
+    <col min="17" max="17" width="19.1640625" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="18.6640625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>